<commit_message>
feat: enhance preview endpoint and fix DHU aggregation logic
- Add structured PreviewResponse schema for file preview endpoint
- Fix DHU aggregation to calculate weighted average instead of unweighted
- Update test data to use relative dates instead of fixed future dates
- Add user scope assignment to datasource tests for proper authorization
- Fix datasource creation by adding required factory_id field in tests
</commit_message>
<xml_diff>
--- a/backend/tests/data/Standard_Master_Widget.xlsx
+++ b/backend/tests/data/Standard_Master_Widget.xlsx
@@ -511,7 +511,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-02-12</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -563,7 +563,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-02-13</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -619,7 +619,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-02-14</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -671,7 +671,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-02-15</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -723,7 +723,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-02-16</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">

</xml_diff>